<commit_message>
increased record time even more
</commit_message>
<xml_diff>
--- a/protocol_andy_NoChr_20160502.xlsx
+++ b/protocol_andy_NoChr_20160502.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23670" yWindow="3135" windowWidth="16380" windowHeight="8205"/>
+    <workbookView xWindow="24600" yWindow="3135" windowWidth="16380" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,8 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>685000</v>
+        <f>13*60*1000</f>
+        <v>780000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>